<commit_message>
added missing N number for new arm and mim schema
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_210_1/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_210_1/WG_Number_excel_table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="26940" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WG NB" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="159">
   <si>
     <t>Submitter</t>
   </si>
@@ -39,13 +39,478 @@
   </si>
   <si>
     <t>N#</t>
+  </si>
+  <si>
+    <t>ISO 10303-1634 ed5 assembly_component_placement_requirements Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1634 ed5 assembly_component_placement_requirements ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1634 ed5 assembly_component_placement_requirements MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1635 ed3 assembly_functional_interface_requirement Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1635 ed3 assembly_functional_interface_requirement ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1635 ed3 assembly_functional_interface_requirement MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1640 ed4 assembly_module_with_macro_component Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1640 ed4 assembly_module_with_macro_component ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1641 ed4 assembly_module_with_subassembly Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1641 ed4 assembly_module_with_subassembly ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1643 ed4 assembly_module_with_interconnect_component Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1643 ed4 assembly_module_with_interconnect_component ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1643 ed4 assembly_module_with_interconnect_component MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1644 ed4 assembly_module_with_cable_component Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1644 ed4 assembly_module_with_cable_component ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1644 ed4 assembly_module_with_cable_component MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1645 ed4 assembly_module_with_packaged_connector_component Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1645 ed4 assembly_module_with_packaged_connector_component ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1645 ed4 assembly_module_with_packaged_connector_component MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1646 ed5 footprint_definition Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1646 ed5 footprint_definition ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1650 ed5 bare_die Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1650 ed5 bare_die ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1668 ed5 fabrication_joint Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1668 ed5 fabrication_joint ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1670 ed5 fabrication_technology Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1670 ed5 fabrication_technology ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1682 ed5 interconnect_2d_shape Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1682 ed5 interconnect_2d_shape ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1685 ed4 interconnect_module_to_assembly_module_relationship Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1686 ed5 interconnect_module_usage_view Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1686 ed5 interconnect_module_usage_view ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1686 ed5 interconnect_module_usage_view MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1687 ed4 interconnect_module_with_macros Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1687 ed4 interconnect_module_with_macros ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1689 ed5 interconnect_physical_requirement_allocation Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1689 ed5 interconnect_physical_requirement_allocation ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1690 ed4 interconnect_placement_requirements Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1690 ed4 interconnect_placement_requirements ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1692 ed5 land Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1692 ed5 land ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1696 ed5 layered_interconnect_module_3d_design Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1696 ed5 layered_interconnect_module_3d_design ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1698 ed6 layered_interconnect_module_design Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1698 ed6 layered_interconnect_module_design ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1700 ed5 layered_interconnect_module_with_printed_component_design Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1700 ed5 layered_interconnect_module_with_printed_component_design ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1701 ed4 layout_macro_definition Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1701 ed4 layout_macro_definition ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1707 ed6 package Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1707 ed6 package ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1707 ed6 package MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1708 ed3 packaged_connector_model Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1708 ed3 packaged_connector_model ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1710 ed4 packaged_part_black_box_model Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1710 ed4 packaged_part_black_box_model ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1716 ed5 layered_interconnect_complex_template Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1716 ed5 layered_interconnect_complex_template ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1718 ed6 layered_interconnect_simple_template Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1718 ed6 layered_interconnect_simple_template ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1723 ed4 physical_node_requirement_to_implementing_component_allocation Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1723 ed4 physical_node_requirement_to_implementing_component_allocation ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1726 ed4 physical_unit_2d_shape Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1726 ed4 physical_unit_2d_shape ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1726 ed4 physical_unit_2d_shape MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1728 ed5 physical_unit_design_view Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1728 ed5 physical_unit_design_view ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1728 ed5 physical_unit_design_view MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1737 ed5 printed_physical_layout_template Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1737 ed5 printed_physical_layout_template ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1737 ed5 printed_physical_layout_template MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1751 ed3 test_requirement_allocation Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1751 ed3 test_requirement_allocation ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1829 ed1 assembly_module_with_packaged_component Document</t>
+  </si>
+  <si>
+    <t>Aminata Mbengue</t>
+  </si>
+  <si>
+    <t>2017-02-16</t>
+  </si>
+  <si>
+    <t>N9398</t>
+  </si>
+  <si>
+    <t>N9399</t>
+  </si>
+  <si>
+    <t>N9400</t>
+  </si>
+  <si>
+    <t>N9401</t>
+  </si>
+  <si>
+    <t>N9402</t>
+  </si>
+  <si>
+    <t>N9403</t>
+  </si>
+  <si>
+    <t>N9404</t>
+  </si>
+  <si>
+    <t>N9405</t>
+  </si>
+  <si>
+    <t>N9406</t>
+  </si>
+  <si>
+    <t>N9407</t>
+  </si>
+  <si>
+    <t>N9408</t>
+  </si>
+  <si>
+    <t>N9409</t>
+  </si>
+  <si>
+    <t>N9410</t>
+  </si>
+  <si>
+    <t>N9411</t>
+  </si>
+  <si>
+    <t>N9412</t>
+  </si>
+  <si>
+    <t>N9413</t>
+  </si>
+  <si>
+    <t>N9414</t>
+  </si>
+  <si>
+    <t>N9415</t>
+  </si>
+  <si>
+    <t>N9416</t>
+  </si>
+  <si>
+    <t>N9417</t>
+  </si>
+  <si>
+    <t>N9418</t>
+  </si>
+  <si>
+    <t>N9419</t>
+  </si>
+  <si>
+    <t>N9420</t>
+  </si>
+  <si>
+    <t>N9421</t>
+  </si>
+  <si>
+    <t>N9422</t>
+  </si>
+  <si>
+    <t>N9423</t>
+  </si>
+  <si>
+    <t>N9424</t>
+  </si>
+  <si>
+    <t>N9425</t>
+  </si>
+  <si>
+    <t>N9426</t>
+  </si>
+  <si>
+    <t>N9427</t>
+  </si>
+  <si>
+    <t>N9428</t>
+  </si>
+  <si>
+    <t>N9429</t>
+  </si>
+  <si>
+    <t>N9430</t>
+  </si>
+  <si>
+    <t>N9431</t>
+  </si>
+  <si>
+    <t>N9432</t>
+  </si>
+  <si>
+    <t>N9433</t>
+  </si>
+  <si>
+    <t>N9434</t>
+  </si>
+  <si>
+    <t>N9435</t>
+  </si>
+  <si>
+    <t>N9436</t>
+  </si>
+  <si>
+    <t>N9437</t>
+  </si>
+  <si>
+    <t>N9438</t>
+  </si>
+  <si>
+    <t>N9439</t>
+  </si>
+  <si>
+    <t>N9440</t>
+  </si>
+  <si>
+    <t>N9441</t>
+  </si>
+  <si>
+    <t>N9442</t>
+  </si>
+  <si>
+    <t>N9443</t>
+  </si>
+  <si>
+    <t>N9444</t>
+  </si>
+  <si>
+    <t>N9445</t>
+  </si>
+  <si>
+    <t>N9446</t>
+  </si>
+  <si>
+    <t>N9447</t>
+  </si>
+  <si>
+    <t>N9448</t>
+  </si>
+  <si>
+    <t>N9449</t>
+  </si>
+  <si>
+    <t>N9450</t>
+  </si>
+  <si>
+    <t>N9451</t>
+  </si>
+  <si>
+    <t>N9452</t>
+  </si>
+  <si>
+    <t>N9453</t>
+  </si>
+  <si>
+    <t>N9454</t>
+  </si>
+  <si>
+    <t>N9455</t>
+  </si>
+  <si>
+    <t>N9456</t>
+  </si>
+  <si>
+    <t>N9457</t>
+  </si>
+  <si>
+    <t>N9458</t>
+  </si>
+  <si>
+    <t>N9459</t>
+  </si>
+  <si>
+    <t>N9460</t>
+  </si>
+  <si>
+    <t>N9461</t>
+  </si>
+  <si>
+    <t>N9462</t>
+  </si>
+  <si>
+    <t>N9463</t>
+  </si>
+  <si>
+    <t>N9464</t>
+  </si>
+  <si>
+    <t>N9465</t>
+  </si>
+  <si>
+    <t>N9466</t>
+  </si>
+  <si>
+    <t>N9467</t>
+  </si>
+  <si>
+    <t>N9468</t>
+  </si>
+  <si>
+    <t>N9469</t>
+  </si>
+  <si>
+    <t>N9470</t>
+  </si>
+  <si>
+    <t>N9471</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>2017/03/17</t>
+  </si>
+  <si>
+    <t>ISO 10303-1829 ed1 assembly_module_with_packaged_component ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1829 ed1 assembly_module_with_packaged_component MIM EXPRESS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -68,6 +533,22 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Monaco"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -109,7 +590,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -120,9 +601,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -402,18 +889,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="92.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -428,313 +915,1155 @@
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="A32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="A37" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="A38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>155</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrected human error: pasted part number and not N number in Excel, but Module.xml had the correct N number
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_210_1/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_210_1/WG_Number_excel_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2480" yWindow="-21160" windowWidth="28140" windowHeight="17160" tabRatio="500"/>
+    <workbookView xWindow="3500" yWindow="-21160" windowWidth="28140" windowHeight="17160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WG NB" sheetId="1" r:id="rId1"/>
@@ -545,13 +545,13 @@
     <t>2017/04/12</t>
   </si>
   <si>
-    <t>N1656</t>
-  </si>
-  <si>
     <t>N9536</t>
   </si>
   <si>
     <t>N9537</t>
+  </si>
+  <si>
+    <t>N9535</t>
   </si>
 </sst>
 </file>
@@ -955,13 +955,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="117" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="4" width="12.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="12.5" style="4" customWidth="1"/>
     <col min="5" max="5" width="84.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="4"/>
@@ -2254,7 +2256,7 @@
     </row>
     <row r="81" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>159</v>
@@ -2270,7 +2272,7 @@
     </row>
     <row r="82" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>159</v>
@@ -2286,7 +2288,7 @@
     </row>
     <row r="83" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
last build related files for submission for ballot
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_210_1/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_210_1/WG_Number_excel_table.xlsx
@@ -558,7 +558,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -600,6 +600,11 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val=".SF NS Text"/>
     </font>
   </fonts>
   <fills count="2">
@@ -647,7 +652,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -666,6 +671,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -955,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="117" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="E64" zoomScale="117" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -966,10 +972,11 @@
     <col min="3" max="4" width="12.5" style="4" customWidth="1"/>
     <col min="5" max="5" width="84.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="57" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -985,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -1000,8 +1007,9 @@
       <c r="F2" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>81</v>
       </c>
@@ -1016,8 +1024,9 @@
       <c r="F3" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
@@ -1032,8 +1041,9 @@
       <c r="F4" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>83</v>
       </c>
@@ -1048,8 +1058,9 @@
       <c r="F5" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>84</v>
       </c>
@@ -1064,8 +1075,9 @@
       <c r="F6" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>85</v>
       </c>
@@ -1080,8 +1092,9 @@
       <c r="F7" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
@@ -1096,8 +1109,9 @@
       <c r="F8" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -1112,8 +1126,9 @@
       <c r="F9" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
@@ -1128,8 +1143,9 @@
       <c r="F10" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
@@ -1144,8 +1160,9 @@
       <c r="F11" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>90</v>
       </c>
@@ -1160,8 +1177,9 @@
       <c r="F12" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
@@ -1176,8 +1194,9 @@
       <c r="F13" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -1192,8 +1211,9 @@
       <c r="F14" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
@@ -1208,8 +1228,9 @@
       <c r="F15" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
@@ -1224,8 +1245,9 @@
       <c r="F16" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>95</v>
       </c>
@@ -1240,8 +1262,9 @@
       <c r="F17" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>96</v>
       </c>
@@ -1256,8 +1279,9 @@
       <c r="F18" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>97</v>
       </c>
@@ -1272,8 +1296,9 @@
       <c r="F19" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>98</v>
       </c>
@@ -1288,8 +1313,9 @@
       <c r="F20" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>99</v>
       </c>
@@ -1304,8 +1330,9 @@
       <c r="F21" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>100</v>
       </c>
@@ -1320,8 +1347,9 @@
       <c r="F22" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>101</v>
       </c>
@@ -1336,8 +1364,9 @@
       <c r="F23" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>102</v>
       </c>
@@ -1352,26 +1381,28 @@
       <c r="F24" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>78</v>
@@ -1379,15 +1410,16 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>78</v>
@@ -1395,15 +1427,16 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>78</v>
@@ -1411,15 +1444,16 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>78</v>
@@ -1427,15 +1461,16 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>78</v>
@@ -1443,15 +1478,16 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>78</v>
@@ -1459,15 +1495,16 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>78</v>
@@ -1475,15 +1512,16 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>78</v>
@@ -1491,15 +1529,16 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>78</v>
@@ -1507,15 +1546,16 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>78</v>
@@ -1523,15 +1563,16 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>78</v>
@@ -1539,15 +1580,16 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>78</v>
@@ -1555,15 +1597,16 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>78</v>
@@ -1571,15 +1614,16 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>78</v>
@@ -1587,31 +1631,33 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
+      <c r="F40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>78</v>
@@ -1619,15 +1665,16 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>78</v>
@@ -1635,15 +1682,16 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>78</v>
@@ -1651,15 +1699,16 @@
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>78</v>
@@ -1667,15 +1716,16 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>78</v>
@@ -1683,15 +1733,16 @@
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>78</v>
@@ -1699,15 +1750,16 @@
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>78</v>
@@ -1715,15 +1767,16 @@
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>78</v>
@@ -1731,15 +1784,16 @@
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>78</v>
@@ -1747,15 +1801,16 @@
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>78</v>
@@ -1763,15 +1818,16 @@
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>78</v>
@@ -1779,15 +1835,16 @@
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>78</v>
@@ -1795,15 +1852,16 @@
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>78</v>
@@ -1811,15 +1869,16 @@
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>78</v>
@@ -1827,15 +1886,16 @@
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>78</v>
@@ -1843,15 +1903,16 @@
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>78</v>
@@ -1859,15 +1920,16 @@
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>78</v>
@@ -1875,15 +1937,16 @@
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>78</v>
@@ -1891,15 +1954,16 @@
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G58" s="10"/>
+    </row>
+    <row r="59" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>78</v>
@@ -1907,15 +1971,16 @@
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G59" s="10"/>
+    </row>
+    <row r="60" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>78</v>
@@ -1923,15 +1988,16 @@
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G60" s="10"/>
+    </row>
+    <row r="61" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>78</v>
@@ -1939,15 +2005,16 @@
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G61" s="10"/>
+    </row>
+    <row r="62" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>78</v>
@@ -1955,15 +2022,16 @@
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G62" s="10"/>
+    </row>
+    <row r="63" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>78</v>
@@ -1971,15 +2039,16 @@
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G63" s="10"/>
+    </row>
+    <row r="64" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>78</v>
@@ -1987,15 +2056,16 @@
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
       <c r="E64" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G64" s="10"/>
     </row>
     <row r="65" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>78</v>
@@ -2003,15 +2073,16 @@
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G65" s="10"/>
     </row>
     <row r="66" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>78</v>
@@ -2019,15 +2090,16 @@
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G66" s="10"/>
     </row>
     <row r="67" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>78</v>
@@ -2035,15 +2107,16 @@
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G67" s="10"/>
     </row>
     <row r="68" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>78</v>
@@ -2051,15 +2124,16 @@
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
       <c r="E68" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G68" s="10"/>
     </row>
     <row r="69" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>78</v>
@@ -2067,15 +2141,16 @@
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G69" s="10"/>
     </row>
     <row r="70" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>78</v>
@@ -2083,15 +2158,16 @@
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
       <c r="E70" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G70" s="10"/>
     </row>
     <row r="71" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>78</v>
@@ -2099,15 +2175,16 @@
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
       <c r="E71" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G71" s="10"/>
     </row>
     <row r="72" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>78</v>
@@ -2115,15 +2192,16 @@
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
       <c r="E72" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G72" s="10"/>
     </row>
     <row r="73" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>78</v>
@@ -2131,15 +2209,16 @@
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G73" s="10"/>
     </row>
     <row r="74" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>78</v>
@@ -2147,15 +2226,16 @@
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G74" s="10"/>
     </row>
     <row r="75" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>78</v>
@@ -2163,15 +2243,16 @@
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="G75" s="10"/>
     </row>
     <row r="76" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>78</v>
@@ -2179,16 +2260,16 @@
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="5" t="s">
-        <v>154</v>
+        <v>77</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G76" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="G76" s="10"/>
     </row>
     <row r="77" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>78</v>
@@ -2196,33 +2277,33 @@
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G77" s="7"/>
+      <c r="G77" s="10"/>
     </row>
     <row r="78" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>159</v>
+        <v>78</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G78" s="7"/>
+        <v>158</v>
+      </c>
+      <c r="G78" s="10"/>
     </row>
     <row r="79" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>159</v>
@@ -2230,7 +2311,7 @@
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>164</v>
@@ -2239,7 +2320,7 @@
     </row>
     <row r="80" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>159</v>
@@ -2247,16 +2328,16 @@
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>159</v>
@@ -2264,13 +2345,14 @@
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>168</v>
+      </c>
+      <c r="G81" s="7"/>
+    </row>
+    <row r="82" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>172</v>
       </c>
@@ -2286,7 +2368,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>173</v>
       </c>

</xml_diff>